<commit_message>
Implementation of validity tot_tut
</commit_message>
<xml_diff>
--- a/Tables/baseline_survey.xlsx
+++ b/Tables/baseline_survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FB26B1-9EDB-46DF-834F-868F2CA2F994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6499B7EA-C16E-43E6-A091-77EAB36B2C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transcribed" sheetId="2" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>(a) Inherite, (b) a gift, (c) bought by me, (d) lend to me, (e) other ____________</t>
   </si>
   <si>
-    <t>How much would you sell the item you want to pawn for?       ______________ pesos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gender      </t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>In the last 6 months, has it happened that at some point you lacked money to pay</t>
+  </si>
+  <si>
+    <t>How much do you think the item you plan to pawn is worth?       ______________ pesos</t>
   </si>
 </sst>
 </file>
@@ -590,22 +590,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5EE0F8-618B-402A-949C-95760694EBA3}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection sqref="A1:B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="110.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -613,398 +613,398 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>10</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>14</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>16</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>17</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>18</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>19</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>20</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>21</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>22</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>23</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>24</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>25</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>26</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>27</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>28</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>29</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>30</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="6"/>
       <c r="B58" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepare for restud submission
</commit_message>
<xml_diff>
--- a/Tables/baseline_survey.xlsx
+++ b/Tables/baseline_survey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6499B7EA-C16E-43E6-A091-77EAB36B2C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF03528E-A094-41F5-ACA7-EFA6706298C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>(d) Need the money for some non urgent expense.</t>
   </si>
   <si>
-    <t>How stressed do you feel from the situation that led to to pawn?</t>
-  </si>
-  <si>
     <t xml:space="preserve">(a) very stressed, (b) somwhat stressed, (c) a little stressed, (d) not stressed </t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>How much do you think the item you plan to pawn is worth?       ______________ pesos</t>
+  </si>
+  <si>
+    <t>How stressed do you feel from the situation that led to pawn?</t>
   </si>
 </sst>
 </file>
@@ -214,12 +214,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -254,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -274,6 +280,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,9 +305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -332,7 +345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -438,7 +451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -580,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -590,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5EE0F8-618B-402A-949C-95760694EBA3}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection sqref="A1:B58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B58" sqref="A1:B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,40 +633,40 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>43</v>
+      <c r="B4" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>50</v>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -682,14 +695,14 @@
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="9">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -700,10 +713,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -714,18 +727,18 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="A17" s="9">
         <v>10</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="9">
         <v>11</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -768,39 +781,39 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="A25" s="9">
         <v>13</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>20</v>
+      <c r="B25" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="9">
+        <v>14</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
-        <v>14</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
+      <c r="A29" s="9">
         <v>15</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>23</v>
+      <c r="B29" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -810,57 +823,57 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
+      <c r="A31" s="9">
         <v>16</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>24</v>
+      <c r="B31" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
+      <c r="A33" s="9">
         <v>17</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>48</v>
+      <c r="B33" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="9">
+        <v>18</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
-        <v>18</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -874,7 +887,7 @@
         <v>19</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -884,11 +897,11 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
+      <c r="A42" s="9">
         <v>20</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>30</v>
+      <c r="B42" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -898,11 +911,11 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
+      <c r="A44" s="9">
         <v>21</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>31</v>
+      <c r="B44" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -912,11 +925,11 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="2">
+      <c r="A46" s="9">
         <v>22</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>32</v>
+      <c r="B46" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -926,19 +939,19 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="2">
+      <c r="A48" s="9">
         <v>23</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="9">
+        <v>24</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="2">
-        <v>24</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -946,7 +959,7 @@
         <v>25</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -954,51 +967,51 @@
         <v>26</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="9">
+        <v>27</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
-        <v>27</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="2">
+      <c r="A54" s="9">
         <v>28</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>49</v>
+      <c r="B54" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="9">
+        <v>29</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="2">
-        <v>29</v>
-      </c>
-      <c r="B56" s="3" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="9">
+        <v>30</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="2">
-        <v>30</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>